<commit_message>
Changed tcl file to correct freq
</commit_message>
<xml_diff>
--- a/Project Optimization.xlsx
+++ b/Project Optimization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\16 Fall 2024\ECE M216A CS M258A\Project\216A_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049FB65A-7E14-447E-A202-06E0EDC120C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADF202E-C8FA-4077-ACBB-D7221400551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9465" yWindow="8580" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -201,15 +201,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,23 +485,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.7109375" style="13" customWidth="1"/>
+    <col min="1" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
     <col min="5" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="2" customWidth="1"/>
-    <col min="10" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="19" customWidth="1"/>
-    <col min="15" max="16" width="10.7109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="10" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="13" customWidth="1"/>
+    <col min="15" max="17" width="10.7109375" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -550,7 +543,7 @@
       <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="11" t="s">
         <v>15</v>
       </c>
       <c r="O1" s="4" t="s">
@@ -567,19 +560,19 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2">
         <f>1/A2</f>
         <v>0.5</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2">
         <f>B2*10^3</f>
         <v>500</v>
       </c>
       <c r="D2" s="2">
-        <f>B2*10^9</f>
+        <f t="shared" ref="D2:D20" si="0">B2*10^9</f>
         <v>500000000</v>
       </c>
       <c r="E2">
@@ -606,18 +599,18 @@
       <c r="L2" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="1">
         <v>9030</v>
       </c>
-      <c r="N2" s="18">
+      <c r="N2" s="12">
         <f>J2+K2</f>
         <v>1142.6600000000001</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="1">
         <f>N2*10^6</f>
         <v>1142660000</v>
       </c>
-      <c r="P2" s="11">
+      <c r="P2" s="1">
         <f>O2/D2</f>
         <v>2.28532</v>
       </c>
@@ -631,19 +624,19 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+      <c r="A3">
         <v>1.9</v>
       </c>
-      <c r="B3" s="13">
-        <f t="shared" ref="B3:B20" si="0">1/A3</f>
+      <c r="B3">
+        <f t="shared" ref="B3:B20" si="1">1/A3</f>
         <v>0.52631578947368418</v>
       </c>
-      <c r="C3" s="13">
-        <f t="shared" ref="C3:C31" si="1">B3*10^3</f>
+      <c r="C3">
+        <f t="shared" ref="C3:C33" si="2">B3*10^3</f>
         <v>526.31578947368416</v>
       </c>
       <c r="D3" s="2">
-        <f>B3*10^9</f>
+        <f t="shared" si="0"/>
         <v>526315789.47368419</v>
       </c>
       <c r="E3">
@@ -670,19 +663,19 @@
       <c r="L3" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="1">
         <v>9090</v>
       </c>
-      <c r="N3" s="18">
-        <f t="shared" ref="N3:N31" si="2">J3+K3</f>
+      <c r="N3" s="12">
+        <f t="shared" ref="N3:N33" si="3">J3+K3</f>
         <v>1203.326</v>
       </c>
-      <c r="O3" s="11">
-        <f t="shared" ref="O3:O31" si="3">N3*10^6</f>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O33" si="4">N3*10^6</f>
         <v>1203326000</v>
       </c>
-      <c r="P3" s="11">
-        <f t="shared" ref="P3:P31" si="4">O3/D3</f>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P33" si="5">O3/D3</f>
         <v>2.2863194</v>
       </c>
       <c r="Q3">
@@ -690,24 +683,24 @@
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1">
-        <f t="shared" ref="T3:T31" si="5">P3*I3/D3</f>
+        <f t="shared" ref="T3:T33" si="6">P3*I3/D3</f>
         <v>1.86540157701188E-5</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
+      <c r="A4">
         <v>1.8</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>555.55555555555554</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C4" s="13">
-        <f t="shared" si="1"/>
-        <v>555.55555555555554</v>
-      </c>
-      <c r="D4" s="2">
-        <f>B4*10^9</f>
         <v>555555555.55555558</v>
       </c>
       <c r="E4">
@@ -734,19 +727,19 @@
       <c r="L4" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="1">
         <v>9160</v>
       </c>
-      <c r="N4" s="18">
-        <f t="shared" si="2"/>
+      <c r="N4" s="12">
+        <f t="shared" si="3"/>
         <v>1274.067</v>
       </c>
-      <c r="O4" s="11">
-        <f t="shared" si="3"/>
+      <c r="O4" s="1">
+        <f t="shared" si="4"/>
         <v>1274067000</v>
       </c>
-      <c r="P4" s="11">
-        <f t="shared" si="4"/>
+      <c r="P4" s="1">
+        <f t="shared" si="5"/>
         <v>2.2933205999999999</v>
       </c>
       <c r="Q4">
@@ -754,24 +747,24 @@
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7726341608265542E-5</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5">
         <v>1.7</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>588.23529411764707</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0.58823529411764708</v>
-      </c>
-      <c r="C5" s="13">
-        <f t="shared" si="1"/>
-        <v>588.23529411764707</v>
-      </c>
-      <c r="D5" s="2">
-        <f>B5*10^9</f>
         <v>588235294.11764705</v>
       </c>
       <c r="E5">
@@ -798,19 +791,19 @@
       <c r="L5" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="1">
         <v>9230</v>
       </c>
-      <c r="N5" s="18">
-        <f t="shared" si="2"/>
+      <c r="N5" s="12">
+        <f t="shared" si="3"/>
         <v>1344.894</v>
       </c>
-      <c r="O5" s="11">
-        <f t="shared" si="3"/>
+      <c r="O5" s="1">
+        <f t="shared" si="4"/>
         <v>1344894000</v>
       </c>
-      <c r="P5" s="11">
-        <f t="shared" si="4"/>
+      <c r="P5" s="1">
+        <f t="shared" si="5"/>
         <v>2.2863198000000002</v>
       </c>
       <c r="Q5">
@@ -818,24 +811,24 @@
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6690438082790982E-5</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6">
         <v>1.6</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>625</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>0.625</v>
-      </c>
-      <c r="C6" s="13">
-        <f t="shared" si="1"/>
-        <v>625</v>
-      </c>
-      <c r="D6" s="2">
-        <f>B6*10^9</f>
         <v>625000000</v>
       </c>
       <c r="E6">
@@ -862,19 +855,19 @@
       <c r="L6" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="1">
         <v>9320</v>
       </c>
-      <c r="N6" s="18">
-        <f t="shared" si="2"/>
+      <c r="N6" s="12">
+        <f t="shared" si="3"/>
         <v>1425.825</v>
       </c>
-      <c r="O6" s="11">
-        <f t="shared" si="3"/>
+      <c r="O6" s="1">
+        <f t="shared" si="4"/>
         <v>1425825000</v>
       </c>
-      <c r="P6" s="11">
-        <f t="shared" si="4"/>
+      <c r="P6" s="1">
+        <f t="shared" si="5"/>
         <v>2.28132</v>
       </c>
       <c r="Q6">
@@ -882,24 +875,24 @@
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5674295415523328E-5</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7">
         <v>1.5</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C7" s="13">
-        <f t="shared" si="1"/>
-        <v>666.66666666666663</v>
-      </c>
-      <c r="D7" s="2">
-        <f>B7*10^9</f>
         <v>666666666.66666663</v>
       </c>
       <c r="E7">
@@ -926,19 +919,19 @@
       <c r="L7" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="1">
         <v>9410</v>
       </c>
-      <c r="N7" s="18">
-        <f t="shared" si="2"/>
+      <c r="N7" s="12">
+        <f t="shared" si="3"/>
         <v>1526.88</v>
       </c>
-      <c r="O7" s="11">
-        <f t="shared" si="3"/>
+      <c r="O7" s="1">
+        <f t="shared" si="4"/>
         <v>1526880000</v>
       </c>
-      <c r="P7" s="11">
-        <f t="shared" si="4"/>
+      <c r="P7" s="1">
+        <f t="shared" si="5"/>
         <v>2.2903200000000004</v>
       </c>
       <c r="Q7">
@@ -946,24 +939,24 @@
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4752623594597122E-5</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8">
         <v>1.4</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>714.28571428571433</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="C8" s="13">
-        <f t="shared" si="1"/>
-        <v>714.28571428571433</v>
-      </c>
-      <c r="D8" s="2">
-        <f>B8*10^9</f>
         <v>714285714.28571427</v>
       </c>
       <c r="E8">
@@ -990,19 +983,19 @@
       <c r="L8" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="1">
         <v>9520</v>
       </c>
-      <c r="N8" s="18">
-        <f t="shared" si="2"/>
+      <c r="N8" s="12">
+        <f t="shared" si="3"/>
         <v>1638.086</v>
       </c>
-      <c r="O8" s="11">
-        <f t="shared" si="3"/>
+      <c r="O8" s="1">
+        <f t="shared" si="4"/>
         <v>1638086000</v>
       </c>
-      <c r="P8" s="11">
-        <f t="shared" si="4"/>
+      <c r="P8" s="1">
+        <f t="shared" si="5"/>
         <v>2.2933204000000003</v>
       </c>
       <c r="Q8">
@@ -1010,24 +1003,24 @@
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.378715338183173E-5</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9">
         <v>1.3</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076916</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>769.23076923076917</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>0.76923076923076916</v>
-      </c>
-      <c r="C9" s="13">
-        <f t="shared" si="1"/>
-        <v>769.23076923076917</v>
-      </c>
-      <c r="D9" s="2">
-        <f>B9*10^9</f>
         <v>769230769.23076916</v>
       </c>
       <c r="E9">
@@ -1054,19 +1047,19 @@
       <c r="L9" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="1">
         <v>9650</v>
       </c>
-      <c r="N9" s="18">
-        <f t="shared" si="2"/>
+      <c r="N9" s="12">
+        <f t="shared" si="3"/>
         <v>1759.4770000000001</v>
       </c>
-      <c r="O9" s="11">
-        <f t="shared" si="3"/>
+      <c r="O9" s="1">
+        <f t="shared" si="4"/>
         <v>1759477000</v>
       </c>
-      <c r="P9" s="11">
-        <f t="shared" si="4"/>
+      <c r="P9" s="1">
+        <f t="shared" si="5"/>
         <v>2.2873201000000001</v>
       </c>
       <c r="Q9">
@@ -1074,24 +1067,24 @@
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2768860310161352E-5</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10">
         <v>1.2</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>833.33333333333337</v>
+      </c>
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="C10" s="13">
-        <f t="shared" si="1"/>
-        <v>833.33333333333337</v>
-      </c>
-      <c r="D10" s="2">
-        <f>B10*10^9</f>
         <v>833333333.33333337</v>
       </c>
       <c r="E10">
@@ -1118,19 +1111,19 @@
       <c r="L10" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="1">
         <v>9790</v>
       </c>
-      <c r="N10" s="18">
-        <f t="shared" si="2"/>
+      <c r="N10" s="12">
+        <f t="shared" si="3"/>
         <v>1911.1</v>
       </c>
-      <c r="O10" s="11">
-        <f t="shared" si="3"/>
+      <c r="O10" s="1">
+        <f t="shared" si="4"/>
         <v>1911100000</v>
       </c>
-      <c r="P10" s="11">
-        <f t="shared" si="4"/>
+      <c r="P10" s="1">
+        <f t="shared" si="5"/>
         <v>2.29332</v>
       </c>
       <c r="Q10">
@@ -1138,24 +1131,24 @@
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.1817557980356095E-5</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>909.09090909090901</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0.90909090909090906</v>
-      </c>
-      <c r="C11" s="13">
-        <f t="shared" si="1"/>
-        <v>909.09090909090901</v>
-      </c>
-      <c r="D11" s="2">
-        <f>B11*10^9</f>
         <v>909090909.090909</v>
       </c>
       <c r="E11">
@@ -1182,19 +1175,19 @@
       <c r="L11" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="1">
         <v>9970</v>
       </c>
-      <c r="N11" s="18">
-        <f t="shared" si="2"/>
+      <c r="N11" s="12">
+        <f t="shared" si="3"/>
         <v>2083.018</v>
       </c>
-      <c r="O11" s="11">
-        <f t="shared" si="3"/>
+      <c r="O11" s="1">
+        <f t="shared" si="4"/>
         <v>2083018000</v>
       </c>
-      <c r="P11" s="11">
-        <f t="shared" si="4"/>
+      <c r="P11" s="1">
+        <f t="shared" si="5"/>
         <v>2.2913198000000001</v>
       </c>
       <c r="Q11">
@@ -1202,24 +1195,24 @@
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.0823313306633226E-5</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C12" s="13">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="D12" s="2">
-        <f>B12*10^9</f>
         <v>1000000000</v>
       </c>
       <c r="E12">
@@ -1246,19 +1239,19 @@
       <c r="L12" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="1">
         <v>10200</v>
       </c>
-      <c r="N12" s="18">
-        <f t="shared" si="2"/>
+      <c r="N12" s="12">
+        <f t="shared" si="3"/>
         <v>2285.3200000000002</v>
       </c>
-      <c r="O12" s="11">
-        <f t="shared" si="3"/>
+      <c r="O12" s="1">
+        <f t="shared" si="4"/>
         <v>2285320000</v>
       </c>
-      <c r="P12" s="11">
-        <f t="shared" si="4"/>
+      <c r="P12" s="1">
+        <f t="shared" si="5"/>
         <v>2.28532</v>
       </c>
       <c r="Q12">
@@ -1266,24 +1259,24 @@
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9.8136114176780793E-6</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13">
         <v>0.9</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>1111.1111111111111</v>
+      </c>
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>1.1111111111111112</v>
-      </c>
-      <c r="C13" s="13">
-        <f t="shared" si="1"/>
-        <v>1111.1111111111111</v>
-      </c>
-      <c r="D13" s="2">
-        <f>B13*10^9</f>
         <v>1111111111.1111112</v>
       </c>
       <c r="E13">
@@ -1310,19 +1303,19 @@
       <c r="L13" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="1">
         <v>10400</v>
       </c>
-      <c r="N13" s="18">
-        <f t="shared" si="2"/>
+      <c r="N13" s="12">
+        <f t="shared" si="3"/>
         <v>2538.134</v>
       </c>
-      <c r="O13" s="11">
-        <f t="shared" si="3"/>
+      <c r="O13" s="1">
+        <f t="shared" si="4"/>
         <v>2538134000</v>
       </c>
-      <c r="P13" s="11">
-        <f t="shared" si="4"/>
+      <c r="P13" s="1">
+        <f t="shared" si="5"/>
         <v>2.2843206</v>
       </c>
       <c r="Q13">
@@ -1330,24 +1323,24 @@
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.8283878186063736E-6</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14">
         <v>0.8</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>1250</v>
+      </c>
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>1.25</v>
-      </c>
-      <c r="C14" s="13">
-        <f t="shared" si="1"/>
-        <v>1250</v>
-      </c>
-      <c r="D14" s="2">
-        <f>B14*10^9</f>
         <v>1250000000</v>
       </c>
       <c r="E14">
@@ -1374,19 +1367,19 @@
       <c r="L14" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="1">
         <v>10700</v>
       </c>
-      <c r="N14" s="18">
-        <f t="shared" si="2"/>
+      <c r="N14" s="12">
+        <f t="shared" si="3"/>
         <v>2861.65</v>
       </c>
-      <c r="O14" s="11">
-        <f t="shared" si="3"/>
+      <c r="O14" s="1">
+        <f t="shared" si="4"/>
         <v>2861650000</v>
       </c>
-      <c r="P14" s="11">
-        <f t="shared" si="4"/>
+      <c r="P14" s="1">
+        <f t="shared" si="5"/>
         <v>2.28932</v>
       </c>
       <c r="Q14">
@@ -1394,24 +1387,24 @@
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.864630560523263E-6</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15">
         <v>0.7</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>1428.5714285714287</v>
+      </c>
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>1.4285714285714286</v>
-      </c>
-      <c r="C15" s="13">
-        <f t="shared" si="1"/>
-        <v>1428.5714285714287</v>
-      </c>
-      <c r="D15" s="2">
-        <f>B15*10^9</f>
         <v>1428571428.5714285</v>
       </c>
       <c r="E15">
@@ -1438,19 +1431,19 @@
       <c r="L15" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="1">
         <v>11200</v>
       </c>
-      <c r="N15" s="18">
-        <f t="shared" si="2"/>
+      <c r="N15" s="12">
+        <f t="shared" si="3"/>
         <v>3266.172</v>
       </c>
-      <c r="O15" s="11">
-        <f t="shared" si="3"/>
+      <c r="O15" s="1">
+        <f t="shared" si="4"/>
         <v>3266172000</v>
       </c>
-      <c r="P15" s="11">
-        <f t="shared" si="4"/>
+      <c r="P15" s="1">
+        <f t="shared" si="5"/>
         <v>2.2863204000000001</v>
       </c>
       <c r="Q15">
@@ -1458,24 +1451,24 @@
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.8725351317702641E-6</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16">
         <v>0.6</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>1666.6666666666667</v>
+      </c>
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="C16" s="13">
-        <f t="shared" si="1"/>
-        <v>1666.6666666666667</v>
-      </c>
-      <c r="D16" s="2">
-        <f>B16*10^9</f>
         <v>1666666666.6666667</v>
       </c>
       <c r="E16">
@@ -1502,19 +1495,19 @@
       <c r="L16" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="1">
         <v>11700</v>
       </c>
-      <c r="N16" s="18">
-        <f t="shared" si="2"/>
+      <c r="N16" s="12">
+        <f t="shared" si="3"/>
         <v>3812.2</v>
       </c>
-      <c r="O16" s="11">
-        <f t="shared" si="3"/>
+      <c r="O16" s="1">
+        <f t="shared" si="4"/>
         <v>3812200000</v>
       </c>
-      <c r="P16" s="11">
-        <f t="shared" si="4"/>
+      <c r="P16" s="1">
+        <f t="shared" si="5"/>
         <v>2.2873199999999998</v>
       </c>
       <c r="Q16">
@@ -1522,24 +1515,24 @@
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.8933198854996469E-6</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17">
         <v>0.5</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C17" s="13">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-      <c r="D17" s="2">
-        <f>B17*10^9</f>
         <v>2000000000</v>
       </c>
       <c r="E17">
@@ -1566,19 +1559,19 @@
       <c r="L17" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="1">
         <v>12500</v>
       </c>
-      <c r="N17" s="18">
-        <f t="shared" si="2"/>
+      <c r="N17" s="12">
+        <f t="shared" si="3"/>
         <v>4570.5789999999997</v>
       </c>
-      <c r="O17" s="11">
-        <f t="shared" si="3"/>
+      <c r="O17" s="1">
+        <f t="shared" si="4"/>
         <v>4570579000</v>
       </c>
-      <c r="P17" s="11">
-        <f t="shared" si="4"/>
+      <c r="P17" s="1">
+        <f t="shared" si="5"/>
         <v>2.2852895000000002</v>
       </c>
       <c r="Q17">
@@ -1586,24 +1579,24 @@
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.9067402223539441E-6</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18">
         <v>0.4</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="C18" s="13">
-        <f t="shared" si="1"/>
-        <v>2500</v>
-      </c>
-      <c r="D18" s="2">
-        <f>B18*10^9</f>
         <v>2500000000</v>
       </c>
       <c r="E18">
@@ -1630,19 +1623,19 @@
       <c r="L18" s="1">
         <v>8050000000</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="1">
         <v>13800</v>
       </c>
-      <c r="N18" s="18">
-        <f t="shared" si="2"/>
+      <c r="N18" s="12">
+        <f t="shared" si="3"/>
         <v>5773.3270000000002</v>
       </c>
-      <c r="O18" s="11">
-        <f t="shared" si="3"/>
+      <c r="O18" s="1">
+        <f t="shared" si="4"/>
         <v>5773327000</v>
       </c>
-      <c r="P18" s="11">
-        <f t="shared" si="4"/>
+      <c r="P18" s="1">
+        <f t="shared" si="5"/>
         <v>2.3093308000000001</v>
       </c>
       <c r="Q18">
@@ -1650,24 +1643,24 @@
       </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.0078380065058726E-6</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="9">
         <v>0.3</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="9">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>3333.3333333333335</v>
+      </c>
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C19" s="13">
-        <f t="shared" si="1"/>
-        <v>3333.3333333333335</v>
-      </c>
-      <c r="D19" s="2">
-        <f>B19*10^9</f>
         <v>3333333333.3333335</v>
       </c>
       <c r="E19" s="9">
@@ -1694,19 +1687,19 @@
       <c r="L19" s="10">
         <v>7930000000</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="10">
         <v>15600</v>
       </c>
-      <c r="N19" s="18">
-        <f t="shared" si="2"/>
+      <c r="N19" s="12">
+        <f t="shared" si="3"/>
         <v>7714.3879999999999</v>
       </c>
-      <c r="O19" s="11">
-        <f t="shared" si="3"/>
+      <c r="O19" s="1">
+        <f t="shared" si="4"/>
         <v>7714388000</v>
       </c>
-      <c r="P19" s="11">
-        <f t="shared" si="4"/>
+      <c r="P19" s="1">
+        <f t="shared" si="5"/>
         <v>2.3143164000000001</v>
       </c>
       <c r="Q19" s="9">
@@ -1714,24 +1707,24 @@
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.9545238924274269E-6</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="A20">
         <v>0.2</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C20" s="13">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="D20" s="2">
-        <f>B20*10^9</f>
         <v>5000000000</v>
       </c>
       <c r="E20">
@@ -1758,19 +1751,19 @@
       <c r="L20" s="1">
         <v>8340000000</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="1">
         <v>21800</v>
       </c>
-      <c r="N20" s="18">
-        <f t="shared" si="2"/>
+      <c r="N20" s="12">
+        <f t="shared" si="3"/>
         <v>13422.537</v>
       </c>
-      <c r="O20" s="11">
-        <f t="shared" si="3"/>
+      <c r="O20" s="1">
+        <f t="shared" si="4"/>
         <v>13422537000</v>
       </c>
-      <c r="P20" s="11">
-        <f t="shared" si="4"/>
+      <c r="P20" s="1">
+        <f t="shared" si="5"/>
         <v>2.6845074000000002</v>
       </c>
       <c r="Q20">
@@ -1778,7 +1771,7 @@
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.4250129165366398E-6</v>
       </c>
       <c r="U20" t="s">
@@ -1786,29 +1779,26 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N21" s="18"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="T21" s="1"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="A22">
         <f>1/B22</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22">
         <v>1.5</v>
       </c>
-      <c r="C22" s="13">
-        <f t="shared" si="1"/>
+      <c r="C22">
+        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
       <c r="D22" s="2">
-        <f>B22*10^9</f>
+        <f t="shared" ref="D22:D33" si="7">B22*10^9</f>
         <v>1500000000</v>
       </c>
       <c r="E22">
@@ -1835,19 +1825,19 @@
       <c r="L22" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="1">
         <v>11300</v>
       </c>
-      <c r="N22" s="18">
-        <f t="shared" si="2"/>
+      <c r="N22" s="12">
+        <f t="shared" si="3"/>
         <v>3427.98</v>
       </c>
-      <c r="O22" s="11">
-        <f t="shared" si="3"/>
+      <c r="O22" s="1">
+        <f t="shared" si="4"/>
         <v>3427980000</v>
       </c>
-      <c r="P22" s="11">
-        <f t="shared" si="4"/>
+      <c r="P22" s="1">
+        <f t="shared" si="5"/>
         <v>2.28532</v>
       </c>
       <c r="Q22">
@@ -1855,24 +1845,24 @@
       </c>
       <c r="S22" s="1"/>
       <c r="T22" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.5424076117853859E-6</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
-        <f t="shared" ref="A23:A31" si="6">1/B23</f>
+      <c r="A23">
+        <f t="shared" ref="A23:A31" si="8">1/B23</f>
         <v>0.625</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23">
         <v>1.6</v>
       </c>
-      <c r="C23" s="13">
-        <f t="shared" si="1"/>
+      <c r="C23">
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="D23" s="2">
-        <f>B23*10^9</f>
+        <f t="shared" si="7"/>
         <v>1600000000</v>
       </c>
       <c r="E23">
@@ -1899,19 +1889,19 @@
       <c r="L23" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="1">
         <v>11500</v>
       </c>
-      <c r="N23" s="18">
-        <f t="shared" si="2"/>
+      <c r="N23" s="12">
+        <f t="shared" si="3"/>
         <v>3660.5120000000002</v>
       </c>
-      <c r="O23" s="11">
-        <f t="shared" si="3"/>
+      <c r="O23" s="1">
+        <f t="shared" si="4"/>
         <v>3660512000</v>
       </c>
-      <c r="P23" s="11">
-        <f t="shared" si="4"/>
+      <c r="P23" s="1">
+        <f t="shared" si="5"/>
         <v>2.28782</v>
       </c>
       <c r="Q23">
@@ -1919,24 +1909,24 @@
       </c>
       <c r="S23" s="1"/>
       <c r="T23" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.1402168168987995E-6</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
-        <f t="shared" si="6"/>
+      <c r="A24">
+        <f t="shared" si="8"/>
         <v>0.58823529411764708</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24">
         <v>1.7</v>
       </c>
-      <c r="C24" s="13">
-        <f t="shared" si="1"/>
+      <c r="C24">
+        <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="D24" s="2">
-        <f>B24*10^9</f>
+        <f t="shared" si="7"/>
         <v>1700000000</v>
       </c>
       <c r="E24">
@@ -1963,19 +1953,19 @@
       <c r="L24" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="1">
         <v>11800</v>
       </c>
-      <c r="N24" s="18">
-        <f t="shared" si="2"/>
+      <c r="N24" s="12">
+        <f t="shared" si="3"/>
         <v>3893.0439999999999</v>
       </c>
-      <c r="O24" s="11">
-        <f t="shared" si="3"/>
+      <c r="O24" s="1">
+        <f t="shared" si="4"/>
         <v>3893044000</v>
       </c>
-      <c r="P24" s="11">
-        <f t="shared" si="4"/>
+      <c r="P24" s="1">
+        <f t="shared" si="5"/>
         <v>2.2900258823529414</v>
       </c>
       <c r="Q24">
@@ -1983,24 +1973,24 @@
       </c>
       <c r="S24" s="1"/>
       <c r="T24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.7845996456763786E-6</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
-        <f t="shared" si="6"/>
+      <c r="A25">
+        <f t="shared" si="8"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25">
         <v>1.8</v>
       </c>
-      <c r="C25" s="13">
-        <f t="shared" si="1"/>
+      <c r="C25">
+        <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="D25" s="2">
-        <f>B25*10^9</f>
+        <f t="shared" si="7"/>
         <v>1800000000</v>
       </c>
       <c r="E25">
@@ -2027,19 +2017,19 @@
       <c r="L25" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="1">
         <v>12000</v>
       </c>
-      <c r="N25" s="18">
-        <f t="shared" si="2"/>
+      <c r="N25" s="12">
+        <f t="shared" si="3"/>
         <v>4115.576</v>
       </c>
-      <c r="O25" s="11">
-        <f t="shared" si="3"/>
+      <c r="O25" s="1">
+        <f t="shared" si="4"/>
         <v>4115576000</v>
       </c>
-      <c r="P25" s="11">
-        <f t="shared" si="4"/>
+      <c r="P25" s="1">
+        <f t="shared" si="5"/>
         <v>2.2864311111111113</v>
       </c>
       <c r="Q25">
@@ -2047,24 +2037,24 @@
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.4546570812680691E-6</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
-        <f t="shared" si="6"/>
+      <c r="A26">
+        <f t="shared" si="8"/>
         <v>0.52631578947368418</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26">
         <v>1.9</v>
       </c>
-      <c r="C26" s="13">
-        <f t="shared" si="1"/>
+      <c r="C26">
+        <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="D26" s="2">
-        <f>B26*10^9</f>
+        <f t="shared" si="7"/>
         <v>1900000000</v>
       </c>
       <c r="E26">
@@ -2091,19 +2081,19 @@
       <c r="L26" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M26" s="11">
+      <c r="M26" s="1">
         <v>12200</v>
       </c>
-      <c r="N26" s="18">
-        <f t="shared" si="2"/>
+      <c r="N26" s="12">
+        <f t="shared" si="3"/>
         <v>4348.1080000000002</v>
       </c>
-      <c r="O26" s="11">
-        <f t="shared" si="3"/>
+      <c r="O26" s="1">
+        <f t="shared" si="4"/>
         <v>4348108000</v>
       </c>
-      <c r="P26" s="11">
-        <f t="shared" si="4"/>
+      <c r="P26" s="1">
+        <f t="shared" si="5"/>
         <v>2.2884778947368423</v>
       </c>
       <c r="Q26">
@@ -2111,24 +2101,24 @@
       </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1721958083247518E-6</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
-        <f t="shared" si="6"/>
+      <c r="A27">
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" s="13">
-        <f t="shared" si="1"/>
+      <c r="C27">
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="D27" s="2">
-        <f>B27*10^9</f>
+        <f t="shared" si="7"/>
         <v>2000000000</v>
       </c>
       <c r="E27">
@@ -2155,19 +2145,19 @@
       <c r="L27" s="1">
         <v>7890000000</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="1">
         <v>12500</v>
       </c>
-      <c r="N27" s="18">
-        <f t="shared" si="2"/>
+      <c r="N27" s="12">
+        <f t="shared" si="3"/>
         <v>4570.5789999999997</v>
       </c>
-      <c r="O27" s="11">
-        <f t="shared" si="3"/>
+      <c r="O27" s="1">
+        <f t="shared" si="4"/>
         <v>4570579000</v>
       </c>
-      <c r="P27" s="11">
-        <f t="shared" si="4"/>
+      <c r="P27" s="1">
+        <f t="shared" si="5"/>
         <v>2.2852895000000002</v>
       </c>
       <c r="Q27">
@@ -2175,24 +2165,24 @@
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.9067402223539441E-6</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
-        <f t="shared" si="6"/>
+      <c r="A28" s="6">
+        <f t="shared" si="8"/>
         <v>0.47619047619047616</v>
       </c>
-      <c r="B28" s="16">
+      <c r="B28" s="6">
         <v>2.1</v>
       </c>
-      <c r="C28" s="13">
-        <f t="shared" si="1"/>
+      <c r="C28">
+        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="D28" s="2">
-        <f>B28*10^9</f>
+        <f t="shared" si="7"/>
         <v>2100000000</v>
       </c>
       <c r="E28" s="6">
@@ -2219,19 +2209,19 @@
       <c r="L28" s="7">
         <v>7890000000</v>
       </c>
-      <c r="M28" s="14">
+      <c r="M28" s="7">
         <v>12700</v>
       </c>
-      <c r="N28" s="18">
-        <f t="shared" si="2"/>
+      <c r="N28" s="12">
+        <f t="shared" si="3"/>
         <v>4803.1080000000002</v>
       </c>
-      <c r="O28" s="11">
-        <f t="shared" si="3"/>
+      <c r="O28" s="1">
+        <f t="shared" si="4"/>
         <v>4803108000</v>
       </c>
-      <c r="P28" s="11">
-        <f t="shared" si="4"/>
+      <c r="P28" s="1">
+        <f t="shared" si="5"/>
         <v>2.2871942857142855</v>
       </c>
       <c r="Q28" s="6">
@@ -2239,24 +2229,24 @@
       </c>
       <c r="S28" s="7"/>
       <c r="T28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.6769809368644782E-6</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
-        <f t="shared" si="6"/>
+      <c r="A29">
+        <f t="shared" si="8"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C29" s="13">
-        <f t="shared" si="1"/>
+      <c r="C29">
+        <f t="shared" si="2"/>
         <v>2200</v>
       </c>
       <c r="D29" s="2">
-        <f>B29*10^9</f>
+        <f t="shared" si="7"/>
         <v>2200000000</v>
       </c>
       <c r="E29">
@@ -2283,19 +2273,19 @@
       <c r="L29" s="1">
         <v>7900000000</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="1">
         <v>12900</v>
       </c>
-      <c r="N29" s="18">
-        <f t="shared" si="2"/>
+      <c r="N29" s="12">
+        <f t="shared" si="3"/>
         <v>5025.6869999999999</v>
       </c>
-      <c r="O29" s="11">
-        <f t="shared" si="3"/>
+      <c r="O29" s="1">
+        <f t="shared" si="4"/>
         <v>5025687000</v>
       </c>
-      <c r="P29" s="11">
-        <f t="shared" si="4"/>
+      <c r="P29" s="1">
+        <f t="shared" si="5"/>
         <v>2.284403181818182</v>
       </c>
       <c r="Q29">
@@ -2303,24 +2293,24 @@
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.4638285000485341E-6</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
-        <f t="shared" si="6"/>
+      <c r="A30">
+        <f t="shared" si="8"/>
         <v>0.43478260869565222</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C30" s="13">
-        <f t="shared" si="1"/>
+      <c r="C30">
+        <f t="shared" si="2"/>
         <v>2300</v>
       </c>
       <c r="D30" s="2">
-        <f>B30*10^9</f>
+        <f t="shared" si="7"/>
         <v>2300000000</v>
       </c>
       <c r="E30">
@@ -2347,19 +2337,19 @@
       <c r="L30" s="1">
         <v>7950000000</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="1">
         <v>13200</v>
       </c>
-      <c r="N30" s="18">
-        <f t="shared" si="2"/>
+      <c r="N30" s="12">
+        <f t="shared" si="3"/>
         <v>5258.1220000000003</v>
       </c>
-      <c r="O30" s="11">
-        <f t="shared" si="3"/>
+      <c r="O30" s="1">
+        <f t="shared" si="4"/>
         <v>5258122000</v>
       </c>
-      <c r="P30" s="11">
-        <f t="shared" si="4"/>
+      <c r="P30" s="1">
+        <f t="shared" si="5"/>
         <v>2.2861400000000001</v>
       </c>
       <c r="Q30">
@@ -2367,24 +2357,24 @@
       </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.3031108584462268E-6</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
-        <f t="shared" si="6"/>
+      <c r="A31">
+        <f t="shared" si="8"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31">
         <v>2.4</v>
       </c>
-      <c r="C31" s="13">
-        <f t="shared" si="1"/>
+      <c r="C31">
+        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
       <c r="D31" s="2">
-        <f>B31*10^9</f>
+        <f t="shared" si="7"/>
         <v>2400000000</v>
       </c>
       <c r="E31">
@@ -2411,19 +2401,19 @@
       <c r="L31" s="1">
         <v>7920000000</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="1">
         <v>13400</v>
       </c>
-      <c r="N31" s="18">
-        <f t="shared" si="2"/>
+      <c r="N31" s="12">
+        <f t="shared" si="3"/>
         <v>5480.6580000000004</v>
       </c>
-      <c r="O31" s="11">
-        <f t="shared" si="3"/>
+      <c r="O31" s="1">
+        <f t="shared" si="4"/>
         <v>5480658000</v>
       </c>
-      <c r="P31" s="11">
-        <f t="shared" si="4"/>
+      <c r="P31" s="1">
+        <f t="shared" si="5"/>
         <v>2.2836075</v>
       </c>
       <c r="Q31">
@@ -2431,8 +2421,84 @@
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.0886535231734634E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="12"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B33">
+        <v>3.448275862</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>3448.275862</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="7"/>
+        <v>3448275862</v>
+      </c>
+      <c r="E33">
+        <v>1588.654166</v>
+      </c>
+      <c r="F33" s="2">
+        <v>71.668609000000004</v>
+      </c>
+      <c r="G33">
+        <v>1919.2955489999999</v>
+      </c>
+      <c r="H33">
+        <v>759.86486100000002</v>
+      </c>
+      <c r="I33">
+        <v>4267.8145750000003</v>
+      </c>
+      <c r="J33">
+        <v>87.594999999999999</v>
+      </c>
+      <c r="K33" s="14">
+        <v>7900</v>
+      </c>
+      <c r="L33" s="1">
+        <v>7930000000</v>
+      </c>
+      <c r="M33" s="1">
+        <v>15900</v>
+      </c>
+      <c r="N33" s="12">
+        <f t="shared" si="3"/>
+        <v>7987.5950000000003</v>
+      </c>
+      <c r="O33" s="1">
+        <f t="shared" si="4"/>
+        <v>7987595000</v>
+      </c>
+      <c r="P33" s="1">
+        <f t="shared" si="5"/>
+        <v>2.3164025500463281</v>
+      </c>
+      <c r="Q33">
+        <v>0.06</v>
+      </c>
+      <c r="T33" s="1">
+        <f t="shared" si="6"/>
+        <v>2.8669332038072562E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>